<commit_message>
correct check for default number format to look for numXfId=0
</commit_message>
<xml_diff>
--- a/samples/default_num_format_sample.xlsx
+++ b/samples/default_num_format_sample.xlsx
@@ -1057,7 +1057,7 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0">
+      <c r="E2">
         <v>4400</v>
       </c>
     </row>
@@ -1074,7 +1074,7 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E3">
         <v>13000</v>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="0">
+      <c r="E4">
         <v>6000</v>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="0">
+      <c r="E5">
         <v>11000</v>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="0">
+      <c r="E6">
         <v>3100</v>
       </c>
     </row>
@@ -1142,7 +1142,7 @@
       <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="0">
+      <c r="E7">
         <v>2900</v>
       </c>
     </row>
@@ -1159,7 +1159,7 @@
       <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="0">
+      <c r="E8">
         <v>2800</v>
       </c>
     </row>
@@ -1176,7 +1176,7 @@
       <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="0">
+      <c r="E9">
         <v>2600</v>
       </c>
     </row>
@@ -1193,7 +1193,7 @@
       <c r="D10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="0">
+      <c r="E10">
         <v>2500</v>
       </c>
     </row>
@@ -1210,7 +1210,7 @@
       <c r="D11" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="0">
+      <c r="E11">
         <v>6500</v>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
       <c r="D12" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="0">
+      <c r="E12">
         <v>8000</v>
       </c>
     </row>
@@ -1244,7 +1244,7 @@
       <c r="D13" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="0">
+      <c r="E13">
         <v>8200</v>
       </c>
     </row>
@@ -1261,7 +1261,7 @@
       <c r="D14" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="0">
+      <c r="E14">
         <v>7900</v>
       </c>
     </row>
@@ -1278,7 +1278,7 @@
       <c r="D15" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="0">
+      <c r="E15">
         <v>6500</v>
       </c>
     </row>
@@ -1295,7 +1295,7 @@
       <c r="D16" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="0">
+      <c r="E16">
         <v>5800</v>
       </c>
     </row>
@@ -1312,7 +1312,7 @@
       <c r="D17" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="0">
+      <c r="E17">
         <v>3200</v>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       <c r="D18" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="0">
+      <c r="E18">
         <v>2700</v>
       </c>
     </row>
@@ -1346,7 +1346,7 @@
       <c r="D19" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="0">
+      <c r="E19">
         <v>2400</v>
       </c>
     </row>
@@ -1363,7 +1363,7 @@
       <c r="D20" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="0">
+      <c r="E20">
         <v>2200</v>
       </c>
     </row>
@@ -1380,7 +1380,7 @@
       <c r="D21" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="0">
+      <c r="E21">
         <v>3300</v>
       </c>
     </row>
@@ -1397,7 +1397,7 @@
       <c r="D22" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="0">
+      <c r="E22">
         <v>2800</v>
       </c>
     </row>
@@ -1414,7 +1414,7 @@
       <c r="D23" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="0">
+      <c r="E23">
         <v>2500</v>
       </c>
     </row>
@@ -1431,7 +1431,7 @@
       <c r="D24" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="0">
+      <c r="E24">
         <v>2100</v>
       </c>
     </row>
@@ -1448,7 +1448,7 @@
       <c r="D25" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="0">
+      <c r="E25">
         <v>3300</v>
       </c>
     </row>
@@ -1465,7 +1465,7 @@
       <c r="D26" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="0">
+      <c r="E26">
         <v>2900</v>
       </c>
     </row>
@@ -1482,7 +1482,7 @@
       <c r="D27" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="0">
+      <c r="E27">
         <v>2400</v>
       </c>
     </row>
@@ -1499,7 +1499,7 @@
       <c r="D28" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="0">
+      <c r="E28">
         <v>2200</v>
       </c>
     </row>
@@ -1516,7 +1516,7 @@
       <c r="D29" t="s">
         <v>42</v>
       </c>
-      <c r="E29" s="0">
+      <c r="E29">
         <v>3600</v>
       </c>
     </row>
@@ -1533,7 +1533,7 @@
       <c r="D30" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="0">
+      <c r="E30">
         <v>3200</v>
       </c>
     </row>
@@ -1550,7 +1550,7 @@
       <c r="D31" t="s">
         <v>42</v>
       </c>
-      <c r="E31" s="0">
+      <c r="E31">
         <v>2700</v>
       </c>
     </row>
@@ -1567,7 +1567,7 @@
       <c r="D32" t="s">
         <v>42</v>
       </c>
-      <c r="E32" s="0">
+      <c r="E32">
         <v>2500</v>
       </c>
     </row>
@@ -1584,7 +1584,7 @@
       <c r="D33" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="0">
+      <c r="E33">
         <v>3500</v>
       </c>
     </row>
@@ -1601,7 +1601,7 @@
       <c r="D34" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="0">
+      <c r="E34">
         <v>3100</v>
       </c>
     </row>
@@ -1618,7 +1618,7 @@
       <c r="D35" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="0">
+      <c r="E35">
         <v>2600</v>
       </c>
     </row>
@@ -1635,7 +1635,7 @@
       <c r="D36" t="s">
         <v>42</v>
       </c>
-      <c r="E36" s="0">
+      <c r="E36">
         <v>2500</v>
       </c>
     </row>
@@ -1652,7 +1652,7 @@
       <c r="D37" t="s">
         <v>42</v>
       </c>
-      <c r="E37" s="0">
+      <c r="E37">
         <v>3200</v>
       </c>
     </row>
@@ -1669,7 +1669,7 @@
       <c r="D38" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="0">
+      <c r="E38">
         <v>3100</v>
       </c>
     </row>
@@ -1686,7 +1686,7 @@
       <c r="D39" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="0">
+      <c r="E39">
         <v>2500</v>
       </c>
     </row>
@@ -1703,7 +1703,7 @@
       <c r="D40" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="0">
+      <c r="E40">
         <v>2800</v>
       </c>
     </row>
@@ -1720,7 +1720,7 @@
       <c r="D41" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="0">
+      <c r="E41">
         <v>4200</v>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       <c r="D42" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="0">
+      <c r="E42">
         <v>4100</v>
       </c>
     </row>
@@ -1754,7 +1754,7 @@
       <c r="D43" t="s">
         <v>42</v>
       </c>
-      <c r="E43" s="0">
+      <c r="E43">
         <v>3400</v>
       </c>
     </row>
@@ -1771,7 +1771,7 @@
       <c r="D44" t="s">
         <v>42</v>
       </c>
-      <c r="E44" s="0">
+      <c r="E44">
         <v>3000</v>
       </c>
     </row>
@@ -1788,7 +1788,7 @@
       <c r="D45" t="s">
         <v>42</v>
       </c>
-      <c r="E45" s="0">
+      <c r="E45">
         <v>3800</v>
       </c>
     </row>
@@ -1805,7 +1805,7 @@
       <c r="D46" t="s">
         <v>42</v>
       </c>
-      <c r="E46" s="0">
+      <c r="E46">
         <v>3600</v>
       </c>
     </row>
@@ -1822,7 +1822,7 @@
       <c r="D47" t="s">
         <v>42</v>
       </c>
-      <c r="E47" s="0">
+      <c r="E47">
         <v>2900</v>
       </c>
     </row>
@@ -1839,7 +1839,7 @@
       <c r="D48" t="s">
         <v>42</v>
       </c>
-      <c r="E48" s="0">
+      <c r="E48">
         <v>2500</v>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       <c r="D49" t="s">
         <v>42</v>
       </c>
-      <c r="E49" s="0">
+      <c r="E49">
         <v>4000</v>
       </c>
     </row>
@@ -1873,7 +1873,7 @@
       <c r="D50" t="s">
         <v>42</v>
       </c>
-      <c r="E50" s="0">
+      <c r="E50">
         <v>3900</v>
       </c>
     </row>
@@ -1890,7 +1890,7 @@
       <c r="D51" t="s">
         <v>42</v>
       </c>
-      <c r="E51" s="0">
+      <c r="E51">
         <v>3200</v>
       </c>
     </row>
@@ -1907,7 +1907,7 @@
       <c r="D52" t="s">
         <v>42</v>
       </c>
-      <c r="E52" s="0">
+      <c r="E52">
         <v>2800</v>
       </c>
     </row>
@@ -1924,7 +1924,7 @@
       <c r="D53" t="s">
         <v>42</v>
       </c>
-      <c r="E53" s="0">
+      <c r="E53">
         <v>3100</v>
       </c>
     </row>
@@ -1941,7 +1941,7 @@
       <c r="D54" t="s">
         <v>42</v>
       </c>
-      <c r="E54" s="0">
+      <c r="E54">
         <v>3000</v>
       </c>
     </row>
@@ -1958,7 +1958,7 @@
       <c r="D55" t="s">
         <v>42</v>
       </c>
-      <c r="E55" s="0">
+      <c r="E55">
         <v>2600</v>
       </c>
     </row>
@@ -1975,7 +1975,7 @@
       <c r="D56" t="s">
         <v>42</v>
       </c>
-      <c r="E56" s="0">
+      <c r="E56">
         <v>2600</v>
       </c>
     </row>
@@ -1992,7 +1992,7 @@
       <c r="D57" t="s">
         <v>171</v>
       </c>
-      <c r="E57" s="0">
+      <c r="E57">
         <v>9000</v>
       </c>
     </row>
@@ -2009,7 +2009,7 @@
       <c r="D58" t="s">
         <v>171</v>
       </c>
-      <c r="E58" s="0">
+      <c r="E58">
         <v>6000</v>
       </c>
     </row>
@@ -2026,7 +2026,7 @@
       <c r="D59" t="s">
         <v>171</v>
       </c>
-      <c r="E59" s="0">
+      <c r="E59">
         <v>4800</v>
       </c>
     </row>
@@ -2043,7 +2043,7 @@
       <c r="D60" t="s">
         <v>171</v>
       </c>
-      <c r="E60" s="0">
+      <c r="E60">
         <v>4800</v>
       </c>
     </row>
@@ -2060,7 +2060,7 @@
       <c r="D61" t="s">
         <v>171</v>
       </c>
-      <c r="E61" s="0">
+      <c r="E61">
         <v>4200</v>
       </c>
     </row>
@@ -2077,7 +2077,7 @@
       <c r="D62" t="s">
         <v>187</v>
       </c>
-      <c r="E62" s="0">
+      <c r="E62">
         <v>10000</v>
       </c>
     </row>
@@ -2094,7 +2094,7 @@
       <c r="D63" t="s">
         <v>190</v>
       </c>
-      <c r="E63" s="0">
+      <c r="E63">
         <v>14000</v>
       </c>
     </row>
@@ -2111,7 +2111,7 @@
       <c r="D64" t="s">
         <v>190</v>
       </c>
-      <c r="E64" s="0">
+      <c r="E64">
         <v>13500</v>
       </c>
     </row>
@@ -2128,7 +2128,7 @@
       <c r="D65" t="s">
         <v>190</v>
       </c>
-      <c r="E65" s="0">
+      <c r="E65">
         <v>12000</v>
       </c>
     </row>
@@ -2145,7 +2145,7 @@
       <c r="D66" t="s">
         <v>190</v>
       </c>
-      <c r="E66" s="0">
+      <c r="E66">
         <v>11000</v>
       </c>
     </row>
@@ -2162,7 +2162,7 @@
       <c r="D67" t="s">
         <v>190</v>
       </c>
-      <c r="E67" s="0">
+      <c r="E67">
         <v>10500</v>
       </c>
     </row>
@@ -2179,7 +2179,7 @@
       <c r="D68" t="s">
         <v>190</v>
       </c>
-      <c r="E68" s="0">
+      <c r="E68">
         <v>10000</v>
       </c>
     </row>
@@ -2196,7 +2196,7 @@
       <c r="D69" t="s">
         <v>190</v>
       </c>
-      <c r="E69" s="0">
+      <c r="E69">
         <v>9500</v>
       </c>
     </row>
@@ -2213,7 +2213,7 @@
       <c r="D70" t="s">
         <v>190</v>
       </c>
-      <c r="E70" s="0">
+      <c r="E70">
         <v>9000</v>
       </c>
     </row>
@@ -2230,7 +2230,7 @@
       <c r="D71" t="s">
         <v>190</v>
       </c>
-      <c r="E71" s="0">
+      <c r="E71">
         <v>8000</v>
       </c>
     </row>
@@ -2247,7 +2247,7 @@
       <c r="D72" t="s">
         <v>190</v>
       </c>
-      <c r="E72" s="0">
+      <c r="E72">
         <v>7500</v>
       </c>
     </row>
@@ -2264,7 +2264,7 @@
       <c r="D73" t="s">
         <v>190</v>
       </c>
-      <c r="E73" s="0">
+      <c r="E73">
         <v>7000</v>
       </c>
     </row>
@@ -2281,7 +2281,7 @@
       <c r="D74" t="s">
         <v>190</v>
       </c>
-      <c r="E74" s="0">
+      <c r="E74">
         <v>10000</v>
       </c>
     </row>
@@ -2298,7 +2298,7 @@
       <c r="D75" t="s">
         <v>190</v>
       </c>
-      <c r="E75" s="0">
+      <c r="E75">
         <v>9500</v>
       </c>
     </row>
@@ -2315,7 +2315,7 @@
       <c r="D76" t="s">
         <v>190</v>
       </c>
-      <c r="E76" s="0">
+      <c r="E76">
         <v>9000</v>
       </c>
     </row>
@@ -2332,7 +2332,7 @@
       <c r="D77" t="s">
         <v>190</v>
       </c>
-      <c r="E77" s="0">
+      <c r="E77">
         <v>8000</v>
       </c>
     </row>
@@ -2349,7 +2349,7 @@
       <c r="D78" t="s">
         <v>190</v>
       </c>
-      <c r="E78" s="0">
+      <c r="E78">
         <v>7500</v>
       </c>
     </row>
@@ -2366,7 +2366,7 @@
       <c r="D79" t="s">
         <v>190</v>
       </c>
-      <c r="E79" s="0">
+      <c r="E79">
         <v>7000</v>
       </c>
     </row>
@@ -2383,7 +2383,7 @@
       <c r="D80" t="s">
         <v>190</v>
       </c>
-      <c r="E80" s="0">
+      <c r="E80">
         <v>10500</v>
       </c>
     </row>
@@ -2400,7 +2400,7 @@
       <c r="D81" t="s">
         <v>190</v>
       </c>
-      <c r="E81" s="0">
+      <c r="E81">
         <v>9500</v>
       </c>
     </row>
@@ -2417,7 +2417,7 @@
       <c r="D82" t="s">
         <v>190</v>
       </c>
-      <c r="E82" s="0">
+      <c r="E82">
         <v>7200</v>
       </c>
     </row>
@@ -2434,7 +2434,7 @@
       <c r="D83" t="s">
         <v>190</v>
       </c>
-      <c r="E83" s="0">
+      <c r="E83">
         <v>6800</v>
       </c>
     </row>
@@ -2451,7 +2451,7 @@
       <c r="D84" t="s">
         <v>190</v>
       </c>
-      <c r="E84" s="0">
+      <c r="E84">
         <v>6400</v>
       </c>
     </row>
@@ -2468,7 +2468,7 @@
       <c r="D85" t="s">
         <v>190</v>
       </c>
-      <c r="E85" s="0">
+      <c r="E85">
         <v>6200</v>
       </c>
     </row>
@@ -2485,7 +2485,7 @@
       <c r="D86" t="s">
         <v>190</v>
       </c>
-      <c r="E86" s="0">
+      <c r="E86">
         <v>11500</v>
       </c>
     </row>
@@ -2502,7 +2502,7 @@
       <c r="D87" t="s">
         <v>190</v>
       </c>
-      <c r="E87" s="0">
+      <c r="E87">
         <v>10000</v>
       </c>
     </row>
@@ -2519,7 +2519,7 @@
       <c r="D88" t="s">
         <v>190</v>
       </c>
-      <c r="E88" s="0">
+      <c r="E88">
         <v>9600</v>
       </c>
     </row>
@@ -2536,7 +2536,7 @@
       <c r="D89" t="s">
         <v>190</v>
       </c>
-      <c r="E89" s="0">
+      <c r="E89">
         <v>7400</v>
       </c>
     </row>
@@ -2553,7 +2553,7 @@
       <c r="D90" t="s">
         <v>190</v>
       </c>
-      <c r="E90" s="0">
+      <c r="E90">
         <v>7300</v>
       </c>
     </row>
@@ -2570,7 +2570,7 @@
       <c r="D91" t="s">
         <v>190</v>
       </c>
-      <c r="E91" s="0">
+      <c r="E91">
         <v>6100</v>
       </c>
     </row>
@@ -2587,7 +2587,7 @@
       <c r="D92" t="s">
         <v>190</v>
       </c>
-      <c r="E92" s="0">
+      <c r="E92">
         <v>11000</v>
       </c>
     </row>
@@ -2604,7 +2604,7 @@
       <c r="D93" t="s">
         <v>190</v>
       </c>
-      <c r="E93" s="0">
+      <c r="E93">
         <v>8800</v>
       </c>
     </row>
@@ -2621,7 +2621,7 @@
       <c r="D94" t="s">
         <v>190</v>
       </c>
-      <c r="E94" s="0">
+      <c r="E94">
         <v>8600</v>
       </c>
     </row>
@@ -2638,7 +2638,7 @@
       <c r="D95" t="s">
         <v>190</v>
       </c>
-      <c r="E95" s="0">
+      <c r="E95">
         <v>8400</v>
       </c>
     </row>
@@ -2655,7 +2655,7 @@
       <c r="D96" t="s">
         <v>190</v>
       </c>
-      <c r="E96" s="0">
+      <c r="E96">
         <v>6200</v>
       </c>
     </row>
@@ -2672,7 +2672,7 @@
       <c r="D97" t="s">
         <v>283</v>
       </c>
-      <c r="E97" s="0">
+      <c r="E97">
         <v>24000</v>
       </c>
     </row>
@@ -2689,7 +2689,7 @@
       <c r="D98" t="s">
         <v>283</v>
       </c>
-      <c r="E98" s="0">
+      <c r="E98">
         <v>17000</v>
       </c>
     </row>
@@ -2706,7 +2706,7 @@
       <c r="D99" t="s">
         <v>283</v>
       </c>
-      <c r="E99" s="0">
+      <c r="E99">
         <v>17000</v>
       </c>
     </row>
@@ -2723,7 +2723,7 @@
       <c r="D100" t="s">
         <v>293</v>
       </c>
-      <c r="E100" s="0">
+      <c r="E100">
         <v>12008</v>
       </c>
     </row>
@@ -2740,7 +2740,7 @@
       <c r="D101" t="s">
         <v>293</v>
       </c>
-      <c r="E101" s="0">
+      <c r="E101">
         <v>9000</v>
       </c>
     </row>
@@ -2757,7 +2757,7 @@
       <c r="D102" t="s">
         <v>293</v>
       </c>
-      <c r="E102" s="0">
+      <c r="E102">
         <v>8200</v>
       </c>
     </row>
@@ -2774,7 +2774,7 @@
       <c r="D103" t="s">
         <v>293</v>
       </c>
-      <c r="E103" s="0">
+      <c r="E103">
         <v>7700</v>
       </c>
     </row>
@@ -2791,7 +2791,7 @@
       <c r="D104" t="s">
         <v>293</v>
       </c>
-      <c r="E104" s="0">
+      <c r="E104">
         <v>7800</v>
       </c>
     </row>
@@ -2808,7 +2808,7 @@
       <c r="D105" t="s">
         <v>293</v>
       </c>
-      <c r="E105" s="0">
+      <c r="E105">
         <v>6900</v>
       </c>
     </row>
@@ -2825,7 +2825,7 @@
       <c r="D106" t="s">
         <v>311</v>
       </c>
-      <c r="E106" s="0">
+      <c r="E106">
         <v>12008</v>
       </c>
     </row>
@@ -2842,7 +2842,7 @@
       <c r="D107" t="s">
         <v>311</v>
       </c>
-      <c r="E107" s="0">
+      <c r="E107">
         <v>8300</v>
       </c>
     </row>
@@ -2859,7 +2859,7 @@
       <c r="D108" t="s">
         <v>190</v>
       </c>
-      <c r="E108" s="0">
+      <c r="E108">
         <v>123.45</v>
       </c>
     </row>

</xml_diff>